<commit_message>
Add dist folder for github page
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/simon/Sites/chord/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C39DD9-6559-EA43-B69F-8382A9EFD8BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D48CFC8-ACF4-F841-B17A-9443F3590C1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="32720" windowHeight="20540" xr2:uid="{7139B7E8-CBAF-C748-B190-630B9108EA14}"/>
   </bookViews>
@@ -703,13 +703,13 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="111" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A40"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.1640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" style="14" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="14" customWidth="1"/>
     <col min="3" max="3" width="23.33203125" style="14" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.33203125" style="20" customWidth="1"/>
@@ -1257,7 +1257,7 @@
         <v>31</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>33</v>
@@ -1419,7 +1419,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="AG2" s="12" t="str">
         <f>+B33</f>
-        <v>Forschungsergebnisse Eship</v>
+        <v>Eship</v>
       </c>
       <c r="AH2" s="12" t="str">
         <f>+B34</f>
@@ -6606,7 +6606,7 @@
       </c>
       <c r="B33" s="10" t="str">
         <f>IF(Objekte!B32="","",Objekte!B32)</f>
-        <v>Forschungsergebnisse Eship</v>
+        <v>Eship</v>
       </c>
       <c r="C33" s="13" t="str">
         <f t="shared" si="6"/>

</xml_diff>